<commit_message>
Fixing minor mistake that failed if readme.md was in the folder
</commit_message>
<xml_diff>
--- a/venv/src/mainControllerDoc/Kontroller.xlsx
+++ b/venv/src/mainControllerDoc/Kontroller.xlsx
@@ -1,101 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chrma\Desktop\Ny mappe\controlProjects\venv\src\mainControllerDoc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87170900-0A90-4323-8070-A4E0DEDB413B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="p3hTFnSzDZq8A442+SdxnzFRzq9mzKyN7xD6V5JnEa5xeULp4v8M8eKFZFxppk7+Z3dB4RXdrAXt+ZDOv9KXIw==" workbookSaltValue="JhELn6da+6BwOnHVP79k8A==" workbookSpinCount="100000" lockStructure="1"/>
+  <workbookProtection lockStructure="1" workbookAlgorithmName="SHA-512" workbookHashValue="p3hTFnSzDZq8A442+SdxnzFRzq9mzKyN7xD6V5JnEa5xeULp4v8M8eKFZFxppk7+Z3dB4RXdrAXt+ZDOv9KXIw==" workbookSaltValue="JhELn6da+6BwOnHVP79k8A==" workbookSpinCount="100000"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="29895" windowHeight="17505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17505" windowWidth="29895" xWindow="5790" yWindow="9300"/>
   </bookViews>
   <sheets>
-    <sheet name="Controls" sheetId="1" r:id="rId1"/>
-    <sheet name="Controllers" sheetId="2" r:id="rId2"/>
+    <sheet name="Controls" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Controllers" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
-  <si>
-    <t>A 7 Human Resources</t>
-  </si>
-  <si>
-    <t>Control</t>
-  </si>
-  <si>
-    <t>Due</t>
-  </si>
-  <si>
-    <t>Verification</t>
-  </si>
-  <si>
-    <t>Responsible</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Controllers</t>
-  </si>
-  <si>
-    <t>contact</t>
-  </si>
-  <si>
-    <t>Gmail</t>
-  </si>
-  <si>
-    <t>Verify Screening processes</t>
-  </si>
-  <si>
-    <t>Knud Bentsen</t>
-  </si>
-  <si>
-    <t>chr.maints@gmail.com</t>
-  </si>
-  <si>
-    <t>Verify terms and conditions</t>
-  </si>
-  <si>
-    <t>Jens Hansen</t>
-  </si>
-  <si>
-    <t>jensh6247@gmail.com</t>
-  </si>
-  <si>
-    <t>hej</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="DD-MM-YYYY" numFmtId="165"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -111,28 +56,88 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="4">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" name="Link" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -420,159 +425,235 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q4"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A5:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="130" zoomScaleNormal="130">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="20.140625"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="25.140625"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" width="18.28515625"/>
+    <col customWidth="1" max="4" min="4" width="11.28515625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>A 7 Human Resources</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Control</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Due</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Verification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Responsible</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Controllers</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>contact</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Gmail</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Verify Screening processes</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>44721</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Knud Bentsen</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Knud Bentsen</t>
+        </is>
+      </c>
+      <c r="P2" s="1" t="inlineStr">
+        <is>
+          <t>chr.maints@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Verify terms and conditions</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>44710</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Jens Hansen</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Jens Hansen</t>
+        </is>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
+          <t>jensh6247@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="16.5" r="4">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>hej</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>44710</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Knud Bentsen</t>
+        </is>
+      </c>
+      <c r="P4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2">
-        <v>44721</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="O2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2">
-        <v>44710</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2">
-        <v>44710</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P4" s="1"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Teleworking</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>44739</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Knud Bentsen</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="P3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="P2" r:id="rId1"/>
+    <hyperlink ref="P3" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="A1" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="13.42578125"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="21.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Controllers</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>contact</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Knud Bentsen</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>chr.maints@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Jens Hansen</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>jensh6247@gmail.com</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Statistics features was added to script
</commit_message>
<xml_diff>
--- a/venv/src/mainControllerDoc/Kontroller.xlsx
+++ b/venv/src/mainControllerDoc/Kontroller.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection lockStructure="1" workbookAlgorithmName="SHA-512" workbookHashValue="p3hTFnSzDZq8A442+SdxnzFRzq9mzKyN7xD6V5JnEa5xeULp4v8M8eKFZFxppk7+Z3dB4RXdrAXt+ZDOv9KXIw==" workbookSaltValue="JhELn6da+6BwOnHVP79k8A==" workbookSpinCount="100000"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17505" windowWidth="29895" xWindow="5790" yWindow="9300"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17505" windowWidth="29895" xWindow="6090" yWindow="1965"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,9 +17,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="DD-MM-YYYY" numFmtId="165"/>
+  <numFmts count="1">
+    <numFmt formatCode="DD-MM-YYYY" numFmtId="164"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -63,7 +62,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -430,13 +429,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="130" zoomScaleNormal="130">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="20.140625"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="25.140625"/>
@@ -502,7 +501,12 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>44721</v>
+        <v>44725</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -530,7 +534,7 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>44710</v>
+        <v>44741</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -573,15 +577,56 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Teleworking</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>44739</v>
+          <t>Verify Screening processes</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>44724</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>Knud Bentsen</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Verify Screening processes</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>44741</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Knud</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Verify Screening processes</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>44741</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Knud</t>
         </is>
       </c>
     </row>
@@ -607,7 +652,7 @@
       <selection activeCell="A1" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="13.42578125"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="21.7109375"/>

</xml_diff>